<commit_message>
domain model finalize, sprint backlog update
</commit_message>
<xml_diff>
--- a/TutorGroup_Deliverable_4_SprintBacklog.xlsx
+++ b/TutorGroup_Deliverable_4_SprintBacklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahyelle/Desktop/Tutor-Software-Engineering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C276B6-8F66-0342-B162-BDDF306FD65D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517BB463-3332-9046-A9D0-D1C84C6A4AB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37100" yWindow="480" windowWidth="27540" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27980" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Number</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Tasks: create function to show tutor profile at appropriate time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hannah - 100% </t>
+  </si>
+  <si>
+    <t>Chase 40%, Calvin 60%</t>
   </si>
 </sst>
 </file>
@@ -416,7 +422,7 @@
   <dimension ref="A1:Z1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -627,9 +633,11 @@
         <v>2</v>
       </c>
       <c r="E14" s="7">
-        <v>0</v>
-      </c>
-      <c r="F14" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="3"/>
@@ -672,7 +680,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="7">
         <v>0</v>
@@ -715,6 +723,9 @@
     <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="B23" s="6" t="s">
         <v>29</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
sprint review document, final edits
</commit_message>
<xml_diff>
--- a/TutorGroup_Deliverable_4_SprintBacklog.xlsx
+++ b/TutorGroup_Deliverable_4_SprintBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahyelle/Desktop/Tutor-Software-Engineering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517BB463-3332-9046-A9D0-D1C84C6A4AB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96445AE6-C91B-FE4A-8F6E-F21FC8278F74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27980" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Number</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Chase 40%, Calvin 60%</t>
+  </si>
+  <si>
+    <t>Hannah 100%</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
   <dimension ref="A1:Z1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -491,7 +494,9 @@
       <c r="E2" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:26" s="9" customFormat="1" ht="16">
       <c r="A3" s="3"/>

</xml_diff>